<commit_message>
Fonts changed, dont click message button!! Ghulam fix the image issue
</commit_message>
<xml_diff>
--- a/Attendence.xlsx
+++ b/Attendence.xlsx
@@ -646,6 +646,11 @@
           <t>Ghulam Muhammad</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -840,6 +845,11 @@
           <t>Osama Akhtar</t>
         </is>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>

</xml_diff>

<commit_message>
New gui named test.py
</commit_message>
<xml_diff>
--- a/Attendence.xlsx
+++ b/Attendence.xlsx
@@ -344,7 +344,7 @@
       <selection activeCell="A1" sqref="A1:AF30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="25.42578125"/>
   </cols>
@@ -455,6 +455,11 @@
           <t>Ghulam Muhammad</t>
         </is>
       </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -462,6 +467,11 @@
           <t>Muhammad Abdullah Bilal</t>
         </is>
       </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -469,6 +479,11 @@
           <t>Muhammad Umer Zia</t>
         </is>
       </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -476,6 +491,11 @@
           <t>Noor-ul-Huda</t>
         </is>
       </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -500,6 +520,11 @@
           <t>Kainat Agha</t>
         </is>
       </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -507,6 +532,11 @@
           <t>Abdullah Sarfaraz</t>
         </is>
       </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -514,6 +544,11 @@
           <t>Abdullahi Ali</t>
         </is>
       </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -521,6 +556,11 @@
           <t>Ahmed Mushtaq</t>
         </is>
       </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -528,6 +568,11 @@
           <t>Ahmed Rihan</t>
         </is>
       </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -535,6 +580,11 @@
           <t>Ahsan Akbar</t>
         </is>
       </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -542,6 +592,11 @@
           <t>Aliza Qamar</t>
         </is>
       </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -549,6 +604,11 @@
           <t>Furqan Abid</t>
         </is>
       </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -556,6 +616,11 @@
           <t>Ghulam Abbas</t>
         </is>
       </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -563,6 +628,11 @@
           <t>Hamdan Ahmed</t>
         </is>
       </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -570,6 +640,11 @@
           <t>Hamza Imran</t>
         </is>
       </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -577,6 +652,11 @@
           <t>Hasan Ahmed</t>
         </is>
       </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -584,6 +664,11 @@
           <t>Hassan Abid</t>
         </is>
       </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -591,6 +676,11 @@
           <t>Hassan Rehan</t>
         </is>
       </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -598,6 +688,11 @@
           <t>Husnain Ali</t>
         </is>
       </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -605,6 +700,11 @@
           <t>Mahyar Ali</t>
         </is>
       </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -612,6 +712,11 @@
           <t>Moaaz Tameer</t>
         </is>
       </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -619,6 +724,11 @@
           <t>Mohib Ullah Khan</t>
         </is>
       </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -626,6 +736,11 @@
           <t>Muhammad Anas</t>
         </is>
       </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -633,6 +748,11 @@
           <t>Muhammad Faizan</t>
         </is>
       </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -640,6 +760,11 @@
           <t>Raja Rakshak</t>
         </is>
       </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -647,11 +772,21 @@
           <t>Safiullah</t>
         </is>
       </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
           <t>Shaheer Ahmed</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -680,7 +815,7 @@
       <selection activeCell="A1" sqref="A1:AF30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="24.42578125"/>
   </cols>
@@ -1016,7 +1151,7 @@
       <selection activeCell="A1" sqref="A1:AF30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="24.5703125"/>
   </cols>
@@ -1351,7 +1486,7 @@
       <selection activeCell="A1" sqref="A1:AF30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="25"/>
   </cols>
@@ -1687,7 +1822,7 @@
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="24.85546875"/>
   </cols>
@@ -2042,7 +2177,7 @@
       <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="24"/>
   </cols>

</xml_diff>